<commit_message>
excel to two dim array code added
</commit_message>
<xml_diff>
--- a/test_data/OrangeData.xlsx
+++ b/test_data/OrangeData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balaji_Dinakaran\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mine\Company\DHL Oct 2023\automation_workspace\OrangeAutomation\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A09B676-9BEB-424A-9D48-E010054BF5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADD4900-141C-4487-B965-E45C20B4BEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" activeTab="2" xr2:uid="{CBAEC157-378C-4DC3-83CE-6A337DB50FBE}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" activeTab="1" xr2:uid="{CBAEC157-378C-4DC3-83CE-6A337DB50FBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,10 +82,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -441,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51C014C4-7052-427A-B83C-222F58F32F68}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -484,6 +490,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -492,7 +499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7901BB02-2552-42CA-82F5-51A1F61D2383}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>

</xml_diff>